<commit_message>
All static fields of shared classes analyzed completely.
</commit_message>
<xml_diff>
--- a/analyzer/results/references/nonfinals.xlsx
+++ b/analyzer/results/references/nonfinals.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IntelliJ Projects\heap-isolation\analyzer\results\references\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A00C379F-702A-4F15-B752-D680BACFF7FE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFB93675-1CB3-4772-91C3-45A50EE538E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -638,7 +638,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -646,13 +646,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -664,13 +688,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -951,8 +981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="D86" sqref="D86:D87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -983,27 +1013,27 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>153</v>
+        <v>78</v>
       </c>
       <c r="B2" t="s">
-        <v>154</v>
+        <v>79</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>85</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="D3" t="s">
         <v>189</v>
@@ -1011,13 +1041,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>84</v>
+        <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>91</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="D4" t="s">
         <v>189</v>
@@ -1025,41 +1055,41 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>175</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="D5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>74</v>
+        <v>181</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>104</v>
       </c>
       <c r="D6" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>119</v>
+        <v>176</v>
       </c>
       <c r="B7" t="s">
-        <v>92</v>
+        <v>177</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>178</v>
       </c>
       <c r="D7" t="s">
         <v>189</v>
@@ -1067,13 +1097,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
       <c r="B8" t="s">
-        <v>92</v>
+        <v>67</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>55</v>
       </c>
       <c r="D8" t="s">
         <v>189</v>
@@ -1081,38 +1111,38 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>6</v>
+        <v>59</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>60</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>59</v>
       </c>
       <c r="D9" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>84</v>
       </c>
       <c r="B10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C10" t="s">
         <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>148</v>
+        <v>84</v>
       </c>
       <c r="B11" t="s">
-        <v>167</v>
+        <v>91</v>
       </c>
       <c r="C11" t="s">
         <v>8</v>
@@ -1123,13 +1153,13 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>129</v>
+        <v>56</v>
       </c>
       <c r="B12" t="s">
-        <v>130</v>
+        <v>57</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>58</v>
       </c>
       <c r="D12" t="s">
         <v>189</v>
@@ -1137,13 +1167,13 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>44</v>
+        <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D13" t="s">
         <v>189</v>
@@ -1151,13 +1181,13 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>116</v>
       </c>
       <c r="B14" t="s">
-        <v>75</v>
+        <v>144</v>
       </c>
       <c r="C14" t="s">
-        <v>8</v>
+        <v>145</v>
       </c>
       <c r="D14" t="s">
         <v>189</v>
@@ -1165,10 +1195,10 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>119</v>
       </c>
       <c r="B15" t="s">
-        <v>128</v>
+        <v>92</v>
       </c>
       <c r="C15" t="s">
         <v>8</v>
@@ -1179,237 +1209,246 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>119</v>
       </c>
       <c r="B16" t="s">
-        <v>140</v>
+        <v>49</v>
       </c>
       <c r="C16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" t="s">
+        <v>189</v>
+      </c>
+      <c r="E16" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" t="s">
+        <v>92</v>
+      </c>
+      <c r="C17" t="s">
         <v>8</v>
       </c>
-      <c r="D16" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="D17" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" t="s">
+        <v>189</v>
+      </c>
+      <c r="E18" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>87</v>
+      </c>
+      <c r="B19" t="s">
+        <v>88</v>
+      </c>
+      <c r="C19" t="s">
+        <v>87</v>
+      </c>
+      <c r="D19" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>148</v>
+      </c>
+      <c r="B20" t="s">
+        <v>167</v>
+      </c>
+      <c r="C20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>172</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B21" t="s">
         <v>173</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C21" t="s">
         <v>174</v>
       </c>
-      <c r="D17" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>66</v>
-      </c>
-      <c r="B18" t="s">
-        <v>67</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="D21" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>129</v>
+      </c>
+      <c r="B22" t="s">
+        <v>130</v>
+      </c>
+      <c r="C22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>129</v>
+      </c>
+      <c r="B23" t="s">
+        <v>157</v>
+      </c>
+      <c r="C23" t="s">
+        <v>97</v>
+      </c>
+      <c r="D23" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" t="s">
         <v>55</v>
       </c>
-      <c r="D18" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>72</v>
-      </c>
-      <c r="B19" t="s">
-        <v>73</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="D25" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" t="s">
+        <v>62</v>
+      </c>
+      <c r="D26" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>105</v>
+      </c>
+      <c r="B27" t="s">
+        <v>106</v>
+      </c>
+      <c r="C27" t="s">
+        <v>107</v>
+      </c>
+      <c r="D27" t="s">
+        <v>189</v>
+      </c>
+      <c r="E27" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>161</v>
+      </c>
+      <c r="B29" t="s">
+        <v>162</v>
+      </c>
+      <c r="C29" t="s">
         <v>55</v>
       </c>
-      <c r="D19" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>53</v>
-      </c>
-      <c r="B20" t="s">
-        <v>54</v>
-      </c>
-      <c r="C20" t="s">
-        <v>55</v>
-      </c>
-      <c r="D20" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>161</v>
-      </c>
-      <c r="B21" t="s">
-        <v>162</v>
-      </c>
-      <c r="C21" t="s">
-        <v>55</v>
-      </c>
-      <c r="D21" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>30</v>
-      </c>
-      <c r="B22" t="s">
-        <v>158</v>
-      </c>
-      <c r="C22" t="s">
-        <v>55</v>
-      </c>
-      <c r="D22" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>15</v>
-      </c>
-      <c r="B23" t="s">
-        <v>16</v>
-      </c>
-      <c r="C23" t="s">
-        <v>15</v>
-      </c>
-      <c r="D23" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>3</v>
-      </c>
-      <c r="B24" t="s">
-        <v>16</v>
-      </c>
-      <c r="C24" t="s">
-        <v>15</v>
-      </c>
-      <c r="D24" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>35</v>
-      </c>
-      <c r="B25" t="s">
-        <v>36</v>
-      </c>
-      <c r="C25" t="s">
-        <v>35</v>
-      </c>
-      <c r="D25" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>37</v>
-      </c>
-      <c r="B26" t="s">
-        <v>38</v>
-      </c>
-      <c r="C26" t="s">
-        <v>39</v>
-      </c>
-      <c r="D26" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>37</v>
-      </c>
-      <c r="B27" t="s">
-        <v>175</v>
-      </c>
-      <c r="C27" t="s">
-        <v>39</v>
-      </c>
-      <c r="D27" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>59</v>
-      </c>
-      <c r="B28" t="s">
-        <v>60</v>
-      </c>
-      <c r="C28" t="s">
-        <v>59</v>
-      </c>
-      <c r="D28" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>125</v>
-      </c>
-      <c r="B29" t="s">
-        <v>126</v>
-      </c>
-      <c r="C29" t="s">
-        <v>127</v>
-      </c>
       <c r="D29" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>141</v>
+        <v>9</v>
       </c>
       <c r="B30" t="s">
-        <v>182</v>
+        <v>24</v>
       </c>
       <c r="C30" t="s">
-        <v>141</v>
+        <v>25</v>
       </c>
       <c r="D30" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>141</v>
+        <v>9</v>
       </c>
       <c r="B31" t="s">
-        <v>142</v>
+        <v>76</v>
       </c>
       <c r="C31" t="s">
-        <v>143</v>
+        <v>77</v>
       </c>
       <c r="D31" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="B32" t="s">
-        <v>31</v>
+        <v>138</v>
       </c>
       <c r="C32" t="s">
-        <v>32</v>
+        <v>139</v>
       </c>
       <c r="D32" t="s">
         <v>189</v>
@@ -1417,13 +1456,13 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B33" t="s">
-        <v>4</v>
+        <v>51</v>
       </c>
       <c r="C33" t="s">
-        <v>5</v>
+        <v>52</v>
       </c>
       <c r="D33" t="s">
         <v>189</v>
@@ -1431,13 +1470,13 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>97</v>
+        <v>9</v>
       </c>
       <c r="B34" t="s">
-        <v>98</v>
+        <v>40</v>
       </c>
       <c r="C34" t="s">
-        <v>5</v>
+        <v>41</v>
       </c>
       <c r="D34" t="s">
         <v>189</v>
@@ -1445,27 +1484,27 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>72</v>
+        <v>9</v>
       </c>
       <c r="B35" t="s">
-        <v>134</v>
+        <v>155</v>
       </c>
       <c r="C35" t="s">
-        <v>135</v>
+        <v>156</v>
       </c>
       <c r="D35" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>56</v>
+        <v>9</v>
       </c>
       <c r="B36" t="s">
-        <v>57</v>
+        <v>151</v>
       </c>
       <c r="C36" t="s">
-        <v>58</v>
+        <v>152</v>
       </c>
       <c r="D36" t="s">
         <v>189</v>
@@ -1473,83 +1512,83 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B37" t="s">
-        <v>70</v>
+        <v>168</v>
       </c>
       <c r="C37" t="s">
-        <v>71</v>
+        <v>169</v>
       </c>
       <c r="D37" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>87</v>
+        <v>9</v>
       </c>
       <c r="B38" t="s">
-        <v>70</v>
+        <v>28</v>
       </c>
       <c r="C38" t="s">
-        <v>93</v>
+        <v>29</v>
       </c>
       <c r="D38" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B39" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C39" t="s">
-        <v>94</v>
+        <v>18</v>
       </c>
       <c r="D39" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B40" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="C40" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="D40" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>116</v>
+        <v>9</v>
       </c>
       <c r="B41" t="s">
-        <v>117</v>
+        <v>183</v>
       </c>
       <c r="C41" t="s">
-        <v>118</v>
+        <v>184</v>
       </c>
       <c r="D41" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>116</v>
+        <v>9</v>
       </c>
       <c r="B42" t="s">
-        <v>144</v>
+        <v>159</v>
       </c>
       <c r="C42" t="s">
-        <v>145</v>
+        <v>160</v>
       </c>
       <c r="D42" t="s">
         <v>189</v>
@@ -1557,55 +1596,55 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>119</v>
+        <v>9</v>
       </c>
       <c r="B43" t="s">
-        <v>13</v>
+        <v>136</v>
       </c>
       <c r="C43" t="s">
-        <v>120</v>
+        <v>137</v>
       </c>
       <c r="D43" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="B44" t="s">
-        <v>13</v>
+        <v>132</v>
       </c>
       <c r="C44" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
       <c r="D44" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B45" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C45" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D45" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>87</v>
+        <v>9</v>
       </c>
       <c r="B46" t="s">
-        <v>88</v>
+        <v>163</v>
       </c>
       <c r="C46" t="s">
-        <v>87</v>
+        <v>164</v>
       </c>
       <c r="D46" t="s">
         <v>189</v>
@@ -1613,260 +1652,251 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>78</v>
+        <v>9</v>
       </c>
       <c r="B47" t="s">
-        <v>82</v>
+        <v>179</v>
       </c>
       <c r="C47" t="s">
-        <v>83</v>
+        <v>180</v>
       </c>
       <c r="D47" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>122</v>
+        <v>9</v>
       </c>
       <c r="B48" t="s">
-        <v>123</v>
+        <v>165</v>
       </c>
       <c r="C48" t="s">
-        <v>124</v>
+        <v>166</v>
       </c>
       <c r="D48" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="B49" t="s">
-        <v>47</v>
+        <v>114</v>
       </c>
       <c r="C49" t="s">
-        <v>46</v>
+        <v>115</v>
       </c>
       <c r="D49" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>9</v>
+      </c>
+      <c r="B50" t="s">
+        <v>68</v>
+      </c>
+      <c r="C50" t="s">
+        <v>69</v>
+      </c>
+      <c r="D50" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>9</v>
+      </c>
+      <c r="B51" t="s">
+        <v>26</v>
+      </c>
+      <c r="C51" t="s">
+        <v>27</v>
+      </c>
+      <c r="D51" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>9</v>
+      </c>
+      <c r="B52" t="s">
+        <v>146</v>
+      </c>
+      <c r="C52" t="s">
+        <v>147</v>
+      </c>
+      <c r="D52" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>9</v>
+      </c>
+      <c r="B53" t="s">
+        <v>19</v>
+      </c>
+      <c r="C53" t="s">
+        <v>20</v>
+      </c>
+      <c r="D53" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>9</v>
+      </c>
+      <c r="B54" t="s">
+        <v>33</v>
+      </c>
+      <c r="C54" t="s">
+        <v>34</v>
+      </c>
+      <c r="D54" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>9</v>
+      </c>
+      <c r="B55" t="s">
+        <v>100</v>
+      </c>
+      <c r="C55" t="s">
+        <v>101</v>
+      </c>
+      <c r="D55" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>9</v>
+      </c>
+      <c r="B56" t="s">
+        <v>108</v>
+      </c>
+      <c r="C56" t="s">
+        <v>109</v>
+      </c>
+      <c r="D56" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>125</v>
+      </c>
+      <c r="B57" t="s">
+        <v>126</v>
+      </c>
+      <c r="C57" t="s">
+        <v>127</v>
+      </c>
+      <c r="D57" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>21</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B58" t="s">
         <v>22</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C58" t="s">
         <v>23</v>
       </c>
-      <c r="D50" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>148</v>
-      </c>
-      <c r="B51" t="s">
-        <v>149</v>
-      </c>
-      <c r="C51" t="s">
-        <v>150</v>
-      </c>
-      <c r="D51" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>80</v>
-      </c>
-      <c r="B52" t="s">
-        <v>81</v>
-      </c>
-      <c r="C52" t="s">
-        <v>80</v>
-      </c>
-      <c r="D52" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>80</v>
-      </c>
-      <c r="B53" t="s">
-        <v>99</v>
-      </c>
-      <c r="C53" t="s">
-        <v>80</v>
-      </c>
-      <c r="D53" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>80</v>
-      </c>
-      <c r="B54" t="s">
-        <v>131</v>
-      </c>
-      <c r="C54" t="s">
-        <v>80</v>
-      </c>
-      <c r="D54" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>35</v>
-      </c>
-      <c r="B55" t="s">
-        <v>112</v>
-      </c>
-      <c r="C55" t="s">
-        <v>113</v>
-      </c>
-      <c r="D55" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>105</v>
-      </c>
-      <c r="B56" t="s">
-        <v>106</v>
-      </c>
-      <c r="C56" t="s">
-        <v>107</v>
-      </c>
-      <c r="D56" t="s">
-        <v>189</v>
-      </c>
-      <c r="E56" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>3</v>
-      </c>
-      <c r="B57" t="s">
-        <v>89</v>
-      </c>
-      <c r="C57" t="s">
-        <v>90</v>
-      </c>
-      <c r="D57" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>119</v>
-      </c>
-      <c r="B58" t="s">
-        <v>49</v>
-      </c>
-      <c r="C58" t="s">
-        <v>50</v>
-      </c>
       <c r="D58" t="s">
         <v>189</v>
       </c>
-      <c r="E58" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="B59" t="s">
-        <v>49</v>
+        <v>75</v>
       </c>
       <c r="C59" t="s">
-        <v>50</v>
+        <v>8</v>
       </c>
       <c r="D59" t="s">
         <v>189</v>
       </c>
-      <c r="E59" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="B60" t="s">
-        <v>43</v>
+        <v>128</v>
       </c>
       <c r="C60" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="D60" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="B61" t="s">
-        <v>24</v>
+        <v>140</v>
       </c>
       <c r="C61" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="D61" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="B62" t="s">
-        <v>76</v>
+        <v>158</v>
       </c>
       <c r="C62" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="D62" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="B63" t="s">
-        <v>138</v>
+        <v>31</v>
       </c>
       <c r="C63" t="s">
-        <v>139</v>
+        <v>32</v>
       </c>
       <c r="D63" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="B64" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="C64" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="D64" t="s">
         <v>189</v>
@@ -1874,13 +1904,13 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>9</v>
+        <v>97</v>
       </c>
       <c r="B65" t="s">
-        <v>40</v>
+        <v>98</v>
       </c>
       <c r="C65" t="s">
-        <v>41</v>
+        <v>5</v>
       </c>
       <c r="D65" t="s">
         <v>189</v>
@@ -1888,335 +1918,335 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>9</v>
+        <v>148</v>
       </c>
       <c r="B66" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C66" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="D66" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>9</v>
+        <v>78</v>
       </c>
       <c r="B67" t="s">
-        <v>151</v>
+        <v>82</v>
       </c>
       <c r="C67" t="s">
-        <v>152</v>
-      </c>
-      <c r="D67" t="s">
-        <v>189</v>
+        <v>83</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="B68" t="s">
-        <v>168</v>
+        <v>65</v>
       </c>
       <c r="C68" t="s">
-        <v>169</v>
-      </c>
-      <c r="D68" t="s">
-        <v>189</v>
+        <v>8</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>9</v>
+        <v>56</v>
       </c>
       <c r="B69" t="s">
-        <v>28</v>
+        <v>74</v>
       </c>
       <c r="C69" t="s">
-        <v>29</v>
-      </c>
-      <c r="D69" t="s">
-        <v>189</v>
+        <v>8</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B70" t="s">
-        <v>17</v>
+        <v>89</v>
       </c>
       <c r="C70" t="s">
-        <v>18</v>
-      </c>
-      <c r="D70" t="s">
-        <v>189</v>
+        <v>90</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>9</v>
+        <v>72</v>
       </c>
       <c r="B71" t="s">
-        <v>95</v>
+        <v>134</v>
       </c>
       <c r="C71" t="s">
-        <v>96</v>
-      </c>
-      <c r="D71" t="s">
-        <v>189</v>
+        <v>135</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>9</v>
+        <v>116</v>
       </c>
       <c r="B72" t="s">
-        <v>183</v>
+        <v>117</v>
       </c>
       <c r="C72" t="s">
-        <v>184</v>
-      </c>
-      <c r="D72" t="s">
-        <v>189</v>
+        <v>118</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>9</v>
+        <v>119</v>
       </c>
       <c r="B73" t="s">
-        <v>159</v>
+        <v>13</v>
       </c>
       <c r="C73" t="s">
-        <v>160</v>
-      </c>
-      <c r="D73" t="s">
-        <v>189</v>
+        <v>120</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="B74" t="s">
-        <v>136</v>
+        <v>13</v>
       </c>
       <c r="C74" t="s">
-        <v>137</v>
-      </c>
-      <c r="D74" t="s">
-        <v>189</v>
+        <v>120</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B75" t="s">
-        <v>132</v>
+        <v>13</v>
       </c>
       <c r="C75" t="s">
-        <v>133</v>
-      </c>
-      <c r="D75" t="s">
-        <v>189</v>
+        <v>14</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B76" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C76" t="s">
-        <v>11</v>
-      </c>
-      <c r="D76" t="s">
-        <v>189</v>
+        <v>94</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B77" t="s">
-        <v>163</v>
+        <v>110</v>
       </c>
       <c r="C77" t="s">
-        <v>164</v>
-      </c>
-      <c r="D77" t="s">
-        <v>189</v>
+        <v>111</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="B78" t="s">
-        <v>179</v>
+        <v>112</v>
       </c>
       <c r="C78" t="s">
-        <v>180</v>
+        <v>113</v>
       </c>
       <c r="D78" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>9</v>
+        <v>102</v>
       </c>
       <c r="B79" t="s">
-        <v>165</v>
+        <v>103</v>
       </c>
       <c r="C79" t="s">
-        <v>166</v>
+        <v>104</v>
       </c>
       <c r="D79" t="s">
-        <v>189</v>
+        <v>199</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B80" t="s">
-        <v>114</v>
+        <v>7</v>
       </c>
       <c r="C80" t="s">
-        <v>115</v>
-      </c>
-      <c r="D80" t="s">
-        <v>189</v>
+        <v>8</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B81" t="s">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="C81" t="s">
-        <v>69</v>
-      </c>
-      <c r="D81" t="s">
-        <v>189</v>
+        <v>8</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
       <c r="B82" t="s">
-        <v>26</v>
+        <v>81</v>
       </c>
       <c r="C82" t="s">
-        <v>27</v>
-      </c>
-      <c r="D82" t="s">
-        <v>189</v>
+        <v>80</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
       <c r="B83" t="s">
-        <v>146</v>
+        <v>99</v>
       </c>
       <c r="C83" t="s">
-        <v>147</v>
-      </c>
-      <c r="D83" t="s">
-        <v>189</v>
+        <v>80</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>9</v>
+        <v>80</v>
       </c>
       <c r="B84" t="s">
-        <v>19</v>
+        <v>131</v>
       </c>
       <c r="C84" t="s">
-        <v>20</v>
-      </c>
-      <c r="D84" t="s">
-        <v>189</v>
+        <v>80</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>9</v>
+        <v>42</v>
       </c>
       <c r="B85" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="C85" t="s">
-        <v>34</v>
-      </c>
-      <c r="D85" t="s">
-        <v>189</v>
+        <v>42</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B86" t="s">
-        <v>100</v>
+        <v>16</v>
       </c>
       <c r="C86" t="s">
-        <v>101</v>
-      </c>
-      <c r="D86" t="s">
-        <v>189</v>
+        <v>15</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B87" t="s">
-        <v>108</v>
+        <v>16</v>
       </c>
       <c r="C87" t="s">
-        <v>109</v>
-      </c>
-      <c r="D87" t="s">
-        <v>189</v>
+        <v>15</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>176</v>
+        <v>141</v>
       </c>
       <c r="B88" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="C88" t="s">
-        <v>178</v>
+        <v>141</v>
       </c>
       <c r="D88" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>170</v>
+        <v>141</v>
       </c>
       <c r="B89" t="s">
-        <v>171</v>
+        <v>142</v>
       </c>
       <c r="C89" t="s">
-        <v>170</v>
+        <v>143</v>
       </c>
       <c r="D89" t="s">
         <v>194</v>
@@ -2224,69 +2254,69 @@
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>30</v>
+        <v>153</v>
       </c>
       <c r="B90" t="s">
-        <v>63</v>
+        <v>154</v>
       </c>
       <c r="C90" t="s">
-        <v>64</v>
+        <v>8</v>
       </c>
       <c r="D90" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B91" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C91" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="D91" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>37</v>
+        <v>72</v>
       </c>
       <c r="B92" t="s">
-        <v>181</v>
+        <v>121</v>
       </c>
       <c r="C92" t="s">
         <v>104</v>
       </c>
       <c r="D92" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>102</v>
+        <v>122</v>
       </c>
       <c r="B93" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
       <c r="C93" t="s">
-        <v>104</v>
+        <v>124</v>
       </c>
       <c r="D93" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>72</v>
+        <v>170</v>
       </c>
       <c r="B94" t="s">
-        <v>121</v>
+        <v>171</v>
       </c>
       <c r="C94" t="s">
-        <v>104</v>
+        <v>170</v>
       </c>
       <c r="D94" t="s">
         <v>194</v>
@@ -2294,35 +2324,35 @@
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>129</v>
+        <v>12</v>
       </c>
       <c r="B95" t="s">
-        <v>157</v>
+        <v>70</v>
       </c>
       <c r="C95" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="D95" t="s">
-        <v>189</v>
+        <v>198</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>53</v>
+        <v>87</v>
       </c>
       <c r="B96" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="C96" t="s">
-        <v>62</v>
+        <v>93</v>
       </c>
       <c r="D96" t="s">
-        <v>189</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C96">
-    <sortCondition ref="C2:C96"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E96">
+    <sortCondition ref="D2:D96"/>
     <sortCondition ref="A2:A96"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2346,7 +2376,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2385,7 +2415,7 @@
       <c r="C2" t="s">
         <v>186</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>190</v>
       </c>
       <c r="E2" t="s">
@@ -2394,33 +2424,36 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C3" t="s">
-        <v>66</v>
-      </c>
-      <c r="D3" t="s">
-        <v>189</v>
+        <v>127</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>66</v>
       </c>
       <c r="B4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C4" t="s">
-        <v>127</v>
+        <v>66</v>
       </c>
       <c r="D4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:E3">
+    <sortCondition ref="D3"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -2429,7 +2462,7 @@
           <x14:formula1>
             <xm:f>reasons!$A$1:$A$15</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:E4</xm:sqref>
+          <xm:sqref>D2:E2 D3:E4</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
18 validation scenarios implemented.
</commit_message>
<xml_diff>
--- a/analyzer/results/references/nonfinals.xlsx
+++ b/analyzer/results/references/nonfinals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IntelliJ Projects\heap-isolation\analyzer\results\references\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C0AEA68-691A-431B-A1E3-F4204D1EFD71}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8CF7F5F-5EDF-4DCB-96CF-3E972A94F059}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="private" sheetId="1" r:id="rId1"/>
@@ -984,8 +984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E96"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="D83" sqref="D83"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="D81" sqref="D81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2139,8 +2139,8 @@
       <c r="C81" t="s">
         <v>83</v>
       </c>
-      <c r="D81" s="2" t="s">
-        <v>190</v>
+      <c r="D81" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -2378,7 +2378,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8142930C-172E-41F0-9EF5-1CE294825125}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>

</xml_diff>